<commit_message>
Extent Reports Added and changes in xpaths
</commit_message>
<xml_diff>
--- a/src/main/java/com/pgw/qa/testdata/PGW_TestData.xlsx
+++ b/src/main/java/com/pgw/qa/testdata/PGW_TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sai Sharan\eclipse-workspace\PaymentGateway\src\main\java\com\pgw\qa\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6866C96-5210-4BF2-8602-B6BFAA5B5BC9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4636485-0B8C-4BCD-A835-DEB33ACB3104}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="360" windowWidth="20730" windowHeight="11280" xr2:uid="{5F68D99C-8976-4207-9D8D-C9E305F39210}"/>
+    <workbookView xWindow="2340" yWindow="2820" windowWidth="15375" windowHeight="7965" xr2:uid="{5F68D99C-8976-4207-9D8D-C9E305F39210}"/>
   </bookViews>
   <sheets>
     <sheet name="PaymentPage" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>1234567897418523</t>
   </si>
@@ -60,6 +60,12 @@
   </si>
   <si>
     <t>Qty</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>9</t>
   </si>
 </sst>
 </file>
@@ -436,7 +442,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="A4" sqref="A1:C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -469,8 +475,8 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
-        <v>5</v>
+      <c r="A3" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>4</v>
@@ -480,7 +486,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
+      <c r="A4" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B4" s="3" t="s">
@@ -494,7 +500,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:C4" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:C2 A4:C4 A3:C3" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Allure Reports are added
</commit_message>
<xml_diff>
--- a/src/main/java/com/pgw/qa/testdata/PGW_TestData.xlsx
+++ b/src/main/java/com/pgw/qa/testdata/PGW_TestData.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sai Sharan\eclipse-workspace\PaymentGateway\src\main\java\com\pgw\qa\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4636485-0B8C-4BCD-A835-DEB33ACB3104}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3A1AD95-5EC0-4A29-9D52-2B0C8FD38C70}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2820" windowWidth="15375" windowHeight="7965" xr2:uid="{5F68D99C-8976-4207-9D8D-C9E305F39210}"/>
+    <workbookView xWindow="-120" yWindow="360" windowWidth="20730" windowHeight="11280" xr2:uid="{5F68D99C-8976-4207-9D8D-C9E305F39210}"/>
   </bookViews>
   <sheets>
-    <sheet name="PaymentPage" sheetId="1" r:id="rId1"/>
+    <sheet name="PaymentPage" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,39 +33,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
-  <si>
-    <t>1234567897418523</t>
-  </si>
-  <si>
-    <t>cvv</t>
-  </si>
-  <si>
-    <t>card</t>
-  </si>
-  <si>
-    <t>333</t>
-  </si>
-  <si>
-    <t>4567891239638521</t>
-  </si>
-  <si>
-    <t>222</t>
-  </si>
-  <si>
-    <t>7894561239638521</t>
-  </si>
-  <si>
-    <t>111</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Qty</t>
   </si>
   <si>
-    <t>6</t>
+    <t>Card</t>
   </si>
   <si>
-    <t>9</t>
+    <t>CVV</t>
+  </si>
+  <si>
+    <t>1234567897418523</t>
   </si>
 </sst>
 </file>
@@ -89,7 +68,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -97,34 +76,13 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -438,69 +396,47 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E6FF878-944E-4F2C-AB3D-10D6B498FAA4}">
-  <dimension ref="A1:C4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B19C230-4C65-4A79-8A2A-5D6C9F5C9839}">
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A1:C4"/>
+      <selection activeCell="B2" sqref="A1:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.7109375" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" s="3" t="s">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="3">
-        <v>1</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="3" t="s">
+      <c r="A2" s="1">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>7</v>
+      <c r="C2" s="1">
+        <v>235</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:C2 A4:C4 A3:C3" numberStoredAsText="1"/>
+    <ignoredError sqref="B2" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>